<commit_message>
Nearly have OAMR Cpp fix working.
</commit_message>
<xml_diff>
--- a/data-raw/FixedOAMRCharcoalProductionPlants.xlsx
+++ b/data-raw/FixedOAMRCharcoalProductionPlants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/IEATools/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1625552D-180E-1B42-BD13-10B4EAFDE0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F8B0E4-8C9D-BF49-BEF9-953789296811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,9 +58,6 @@
     <t>Charcoal</t>
   </si>
   <si>
-    <t>Total energy supply</t>
-  </si>
-  <si>
     <t xml:space="preserve">      Charcoal production plants</t>
   </si>
   <si>
@@ -137,6 +134,9 @@
   </si>
   <si>
     <t>The Fixed tab provides a data frame that can be used in IEATools::do_fix().</t>
+  </si>
+  <si>
+    <t>Total primary energy supply</t>
   </si>
 </sst>
 </file>
@@ -1008,37 +1008,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1051,7 +1051,7 @@
   <dimension ref="A1:BM6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1387,7 +1387,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1548,7 +1548,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -1706,7 +1706,7 @@
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" t="e">
         <f>D4/-D3</f>
@@ -1919,7 +1919,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A996B8-05AC-1446-AC43-58639BB2DDE4}">
   <dimension ref="A1:BV7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1928,31 +1930,31 @@
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
       </c>
       <c r="J1">
         <v>1971</v>
@@ -2077,31 +2079,31 @@
     </row>
     <row r="2" spans="1:49" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J2" s="3">
         <f>'OAMR IEA WEB 2022'!D2+(-Fixed!J3)</f>
@@ -2266,31 +2268,31 @@
     </row>
     <row r="3" spans="1:49" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J3" s="3">
         <f>-J4/'OAMR IEA WEB 2022'!$AR$6</f>
@@ -2455,31 +2457,31 @@
     </row>
     <row r="4" spans="1:49" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J4" s="2">
         <v>154</v>

</xml_diff>

<commit_message>
OAMR Cpp replacement data frame now correct.
</commit_message>
<xml_diff>
--- a/data-raw/FixedOAMRCharcoalProductionPlants.xlsx
+++ b/data-raw/FixedOAMRCharcoalProductionPlants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/IEATools/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F8B0E4-8C9D-BF49-BEF9-953789296811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E67E47F-C422-DE4E-BD42-5FAF796A2761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -641,7 +641,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -1048,7 +1048,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BM6"/>
+  <dimension ref="A1:BA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1917,10 +1917,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A996B8-05AC-1446-AC43-58639BB2DDE4}">
-  <dimension ref="A1:BV7"/>
+  <dimension ref="A1:AW7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2094,10 +2094,10 @@
         <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Add a Fixed OAMR Gas works file.
</commit_message>
<xml_diff>
--- a/data-raw/FixedOAMRCharcoalProductionPlants.xlsx
+++ b/data-raw/FixedOAMRCharcoalProductionPlants.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/IEATools/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E67E47F-C422-DE4E-BD42-5FAF796A2761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A07BF05-D395-4942-95AA-2613A110B958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="3" r:id="rId1"/>
-    <sheet name="OAMR IEA WEB 2022" sheetId="1" r:id="rId2"/>
+    <sheet name="OAMR Cpp IEA WEB 2022" sheetId="1" r:id="rId2"/>
     <sheet name="Fixed" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -1920,12 +1920,20 @@
   <dimension ref="A1:AW7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="9" width="25" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.2">
@@ -2106,163 +2114,163 @@
         <v>29</v>
       </c>
       <c r="J2" s="3">
-        <f>'OAMR IEA WEB 2022'!D2+(-Fixed!J3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!D2+(-Fixed!J3)</f>
         <v>11843.818181818182</v>
       </c>
       <c r="K2" s="3">
-        <f>'OAMR IEA WEB 2022'!E2+(-Fixed!K3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!E2+(-Fixed!K3)</f>
         <v>9543.818181818182</v>
       </c>
       <c r="L2" s="3">
-        <f>'OAMR IEA WEB 2022'!F2+(-Fixed!L3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!F2+(-Fixed!L3)</f>
         <v>10626.818181818182</v>
       </c>
       <c r="M2" s="3">
-        <f>'OAMR IEA WEB 2022'!G2+(-Fixed!M3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!G2+(-Fixed!M3)</f>
         <v>10086.818181818182</v>
       </c>
       <c r="N2" s="3">
-        <f>'OAMR IEA WEB 2022'!H2+(-Fixed!N3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!H2+(-Fixed!N3)</f>
         <v>9376.818181818182</v>
       </c>
       <c r="O2" s="3">
-        <f>'OAMR IEA WEB 2022'!I2+(-Fixed!O3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!I2+(-Fixed!O3)</f>
         <v>9084.181818181818</v>
       </c>
       <c r="P2" s="3">
-        <f>'OAMR IEA WEB 2022'!J2+(-Fixed!P3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!J2+(-Fixed!P3)</f>
         <v>10049.181818181818</v>
       </c>
       <c r="Q2" s="3">
-        <f>'OAMR IEA WEB 2022'!K2+(-Fixed!Q3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!K2+(-Fixed!Q3)</f>
         <v>9747.181818181818</v>
       </c>
       <c r="R2" s="3">
-        <f>'OAMR IEA WEB 2022'!L2+(-Fixed!R3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!L2+(-Fixed!R3)</f>
         <v>10549.545454545454</v>
       </c>
       <c r="S2" s="3">
-        <f>'OAMR IEA WEB 2022'!M2+(-Fixed!S3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!M2+(-Fixed!S3)</f>
         <v>10676.818181818182</v>
       </c>
       <c r="T2" s="3">
-        <f>'OAMR IEA WEB 2022'!N2+(-Fixed!T3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!N2+(-Fixed!T3)</f>
         <v>9448.818181818182</v>
       </c>
       <c r="U2" s="3">
-        <f>'OAMR IEA WEB 2022'!O2+(-Fixed!U3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!O2+(-Fixed!U3)</f>
         <v>9975.818181818182</v>
       </c>
       <c r="V2" s="3">
-        <f>'OAMR IEA WEB 2022'!P2+(-Fixed!V3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!P2+(-Fixed!V3)</f>
         <v>9523.818181818182</v>
       </c>
       <c r="W2" s="3">
-        <f>'OAMR IEA WEB 2022'!Q2+(-Fixed!W3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!Q2+(-Fixed!W3)</f>
         <v>9349.181818181818</v>
       </c>
       <c r="X2" s="3">
-        <f>'OAMR IEA WEB 2022'!R2+(-Fixed!X3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!R2+(-Fixed!X3)</f>
         <v>9359.181818181818</v>
       </c>
       <c r="Y2" s="3">
-        <f>'OAMR IEA WEB 2022'!S2+(-Fixed!Y3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!S2+(-Fixed!Y3)</f>
         <v>10359.181818181818</v>
       </c>
       <c r="Z2" s="3">
-        <f>'OAMR IEA WEB 2022'!T2+(-Fixed!Z3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!T2+(-Fixed!Z3)</f>
         <v>8713.818181818182</v>
       </c>
       <c r="AA2" s="3">
-        <f>'OAMR IEA WEB 2022'!U2+(-Fixed!AA3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!U2+(-Fixed!AA3)</f>
         <v>9120.181818181818</v>
       </c>
       <c r="AB2" s="3">
-        <f>'OAMR IEA WEB 2022'!V2+(-Fixed!AB3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!V2+(-Fixed!AB3)</f>
         <v>9059.181818181818</v>
       </c>
       <c r="AC2" s="3">
-        <f>'OAMR IEA WEB 2022'!W2+(-Fixed!AC3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!W2+(-Fixed!AC3)</f>
         <v>10755.909090909092</v>
       </c>
       <c r="AD2" s="3">
-        <f>'OAMR IEA WEB 2022'!X2+(-Fixed!AD3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!X2+(-Fixed!AD3)</f>
         <v>11169.545454545454</v>
       </c>
       <c r="AE2" s="3">
-        <f>'OAMR IEA WEB 2022'!Y2+(-Fixed!AE3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!Y2+(-Fixed!AE3)</f>
         <v>10364.545454545454</v>
       </c>
       <c r="AF2" s="3">
-        <f>'OAMR IEA WEB 2022'!Z2+(-Fixed!AF3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!Z2+(-Fixed!AF3)</f>
         <v>10645.545454545454</v>
       </c>
       <c r="AG2" s="3">
-        <f>'OAMR IEA WEB 2022'!AA2+(-Fixed!AG3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!AA2+(-Fixed!AG3)</f>
         <v>10868.545454545454</v>
       </c>
       <c r="AH2" s="3">
-        <f>'OAMR IEA WEB 2022'!AB2+(-Fixed!AH3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!AB2+(-Fixed!AH3)</f>
         <v>11141.545454545454</v>
       </c>
       <c r="AI2" s="3">
-        <f>'OAMR IEA WEB 2022'!AC2+(-Fixed!AI3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!AC2+(-Fixed!AI3)</f>
         <v>11093.909090909092</v>
       </c>
       <c r="AJ2" s="3">
-        <f>'OAMR IEA WEB 2022'!AD2+(-Fixed!AJ3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!AD2+(-Fixed!AJ3)</f>
         <v>12110.272727272728</v>
       </c>
       <c r="AK2" s="3">
-        <f>'OAMR IEA WEB 2022'!AE2+(-Fixed!AK3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!AE2+(-Fixed!AK3)</f>
         <v>11342.272727272728</v>
       </c>
       <c r="AL2" s="3">
-        <f>'OAMR IEA WEB 2022'!AF2+(-Fixed!AL3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!AF2+(-Fixed!AL3)</f>
         <v>11582.272727272728</v>
       </c>
       <c r="AM2" s="3">
-        <f>'OAMR IEA WEB 2022'!AG2+(-Fixed!AM3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!AG2+(-Fixed!AM3)</f>
         <v>10193.636363636364</v>
       </c>
       <c r="AN2" s="3">
-        <f>'OAMR IEA WEB 2022'!AH2+(-Fixed!AN3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!AH2+(-Fixed!AN3)</f>
         <v>9707.636363636364</v>
       </c>
       <c r="AO2" s="3">
-        <f>'OAMR IEA WEB 2022'!AI2+(-Fixed!AO3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!AI2+(-Fixed!AO3)</f>
         <v>9841</v>
       </c>
       <c r="AP2" s="3">
-        <f>'OAMR IEA WEB 2022'!AJ2+(-Fixed!AP3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!AJ2+(-Fixed!AP3)</f>
         <v>9865</v>
       </c>
       <c r="AQ2" s="3">
-        <f>'OAMR IEA WEB 2022'!AK2+(-Fixed!AQ3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!AK2+(-Fixed!AQ3)</f>
         <v>10215</v>
       </c>
       <c r="AR2" s="3">
-        <f>'OAMR IEA WEB 2022'!AL2+(-Fixed!AR3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!AL2+(-Fixed!AR3)</f>
         <v>9727</v>
       </c>
       <c r="AS2" s="3">
-        <f>'OAMR IEA WEB 2022'!AM2+(-Fixed!AS3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!AM2+(-Fixed!AS3)</f>
         <v>9767</v>
       </c>
       <c r="AT2" s="3">
-        <f>'OAMR IEA WEB 2022'!AN2+(-Fixed!AT3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!AN2+(-Fixed!AT3)</f>
         <v>9280</v>
       </c>
       <c r="AU2" s="3">
-        <f>'OAMR IEA WEB 2022'!AO2+(-Fixed!AU3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!AO2+(-Fixed!AU3)</f>
         <v>8670</v>
       </c>
       <c r="AV2" s="3">
-        <f>'OAMR IEA WEB 2022'!AP2+(-Fixed!AV3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!AP2+(-Fixed!AV3)</f>
         <v>8855</v>
       </c>
       <c r="AW2" s="3">
-        <f>'OAMR IEA WEB 2022'!AQ2+(-Fixed!AW3)</f>
+        <f>'OAMR Cpp IEA WEB 2022'!AQ2+(-Fixed!AW3)</f>
         <v>9206</v>
       </c>
     </row>
@@ -2295,163 +2303,163 @@
         <v>29</v>
       </c>
       <c r="J3" s="3">
-        <f>-J4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-J4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-236.81818181818181</v>
       </c>
       <c r="K3" s="3">
-        <f>-K4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-K4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-236.81818181818181</v>
       </c>
       <c r="L3" s="3">
-        <f>-L4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-L4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-236.81818181818181</v>
       </c>
       <c r="M3" s="3">
-        <f>-M4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-M4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-236.81818181818181</v>
       </c>
       <c r="N3" s="3">
-        <f>-N4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-N4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-236.81818181818181</v>
       </c>
       <c r="O3" s="3">
-        <f>-O4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-O4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-284.18181818181819</v>
       </c>
       <c r="P3" s="3">
-        <f>-P4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-P4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-284.18181818181819</v>
       </c>
       <c r="Q3" s="3">
-        <f>-Q4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-Q4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-284.18181818181819</v>
       </c>
       <c r="R3" s="3">
-        <f>-R4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-R4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-331.54545454545456</v>
       </c>
       <c r="S3" s="3">
-        <f>-S4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-S4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-236.81818181818181</v>
       </c>
       <c r="T3" s="3">
-        <f>-T4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-T4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-236.81818181818181</v>
       </c>
       <c r="U3" s="3">
-        <f>-U4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-U4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-236.81818181818181</v>
       </c>
       <c r="V3" s="3">
-        <f>-V4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-V4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-236.81818181818181</v>
       </c>
       <c r="W3" s="3">
-        <f>-W4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-W4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-284.18181818181819</v>
       </c>
       <c r="X3" s="3">
-        <f>-X4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-X4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-284.18181818181819</v>
       </c>
       <c r="Y3" s="3">
-        <f>-Y4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-Y4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-284.18181818181819</v>
       </c>
       <c r="Z3" s="3">
-        <f>-Z4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-Z4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-236.81818181818181</v>
       </c>
       <c r="AA3" s="3">
-        <f>-AA4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AA4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-284.18181818181819</v>
       </c>
       <c r="AB3" s="3">
-        <f>-AB4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AB4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-284.18181818181819</v>
       </c>
       <c r="AC3" s="3">
-        <f>-AC4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AC4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-899.90909090909099</v>
       </c>
       <c r="AD3" s="3">
-        <f>-AD4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AD4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-852.5454545454545</v>
       </c>
       <c r="AE3" s="3">
-        <f>-AE4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AE4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-852.5454545454545</v>
       </c>
       <c r="AF3" s="3">
-        <f>-AF4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AF4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-852.5454545454545</v>
       </c>
       <c r="AG3" s="3">
-        <f>-AG4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AG4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-852.5454545454545</v>
       </c>
       <c r="AH3" s="3">
-        <f>-AH4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AH4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-852.5454545454545</v>
       </c>
       <c r="AI3" s="3">
-        <f>-AI4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AI4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-899.90909090909099</v>
       </c>
       <c r="AJ3" s="3">
-        <f>-AJ4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AJ4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-947.27272727272725</v>
       </c>
       <c r="AK3" s="3">
-        <f>-AK4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AK4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-947.27272727272725</v>
       </c>
       <c r="AL3" s="3">
-        <f>-AL4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AL4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-947.27272727272725</v>
       </c>
       <c r="AM3" s="3">
-        <f>-AM4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AM4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-994.63636363636363</v>
       </c>
       <c r="AN3" s="3">
-        <f>-AN4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AN4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-994.63636363636363</v>
       </c>
       <c r="AO3" s="3">
-        <f>-AO4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AO4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-1042</v>
       </c>
       <c r="AP3" s="3">
-        <f>-AP4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AP4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-1042</v>
       </c>
       <c r="AQ3" s="3">
-        <f>-AQ4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AQ4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-1042</v>
       </c>
       <c r="AR3" s="3">
-        <f>-AR4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AR4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-1042</v>
       </c>
       <c r="AS3" s="3">
-        <f>-AS4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AS4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-1042</v>
       </c>
       <c r="AT3" s="3">
-        <f>-AT4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AT4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-1042</v>
       </c>
       <c r="AU3" s="3">
-        <f>-AU4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AU4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-1042</v>
       </c>
       <c r="AV3" s="3">
-        <f>-AV4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AV4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-1042</v>
       </c>
       <c r="AW3" s="3">
-        <f>-AW4/'OAMR IEA WEB 2022'!$AR$6</f>
+        <f>-AW4/'OAMR Cpp IEA WEB 2022'!$AR$6</f>
         <v>-1042</v>
       </c>
     </row>

</xml_diff>